<commit_message>
added retour cahier des charges + guidelines pour rapports
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Lecture des conventions de codages Java pour rédaction des conventions de l'équipe</t>
+  </si>
+  <si>
+    <t>Rédaction des conventions à employer pour le code et les commentaires Java</t>
+  </si>
+  <si>
+    <t>Modélisation du schéma relationnel sur papier avec Héléna</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -751,14 +757,26 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
+      <c r="A25" s="3">
+        <v>43170</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>43171</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
@@ -791,7 +809,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>23.25</v>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated gitignore and JdT
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA24088-C302-A643-A6C0-72DE004E989E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB731706-F745-064F-B14D-05F014ACC23C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Implémentation partielle des classes de la BLL BankAccountModel et BankAccountLogic. Commantaires (javadoc) déjà en place</t>
+  </si>
+  <si>
+    <t>Résolution des problèmes liés à une mauvaise utilisation de Maven. Problèmes de dépendances, de version de java, etc.</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,10 +1003,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="8"/>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>43203</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
@@ -1071,7 +1080,7 @@
       </c>
       <c r="C56" s="9">
         <f>SUM(C5:C55)</f>
-        <v>43.25</v>
+        <v>44.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MaJ JdT. Implemented CategoryModel and CategoryLogic. Some changes made to classes already implemented
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE821CD3-DEC1-2A4E-8BCA-D2B05FC55A91}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDDE714-5394-D145-87CB-6CFD65382131}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>Classe Authentication faite partiellement. En attente des fonctions de la DAL pour continuer. Modification de ClientModel et de BankAccount model et logic</t>
+  </si>
+  <si>
+    <t>Préparation de la présentation intermédiaire et présentation</t>
+  </si>
+  <si>
+    <t>Clean du repo git, suppression des fichiers inutilisés</t>
+  </si>
+  <si>
+    <t>Implémentation des classes CategoryModel et CategoryLogic. Adaptation des classes précédemment faites.</t>
   </si>
 </sst>
 </file>
@@ -558,7 +567,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1043,19 +1052,37 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="8"/>
+      <c r="A46" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="8"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="8"/>
+      <c r="A47" s="3">
+        <v>43205</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>43208</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
@@ -1098,7 +1125,7 @@
       </c>
       <c r="C56" s="9">
         <f>SUM(C5:C55)</f>
-        <v>46</v>
+        <v>49.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change G to g in ClientPGEntity.java
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDDE714-5394-D145-87CB-6CFD65382131}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012F4DB-A116-BF42-A76B-596179DDC028}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Implémentation des classes CategoryModel et CategoryLogic. Adaptation des classes précédemment faites.</t>
+  </si>
+  <si>
+    <t>Travail en groupe</t>
+  </si>
+  <si>
+    <t>Travail en groupe via chat vocal</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1085,13 +1091,23 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="8"/>
+      <c r="A49" s="3">
+        <v>43213</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="3">
+        <v>43219</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1125,7 +1141,7 @@
       </c>
       <c r="C56" s="9">
         <f>SUM(C5:C55)</f>
-        <v>49.25</v>
+        <v>50.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started writing report. Updated jdt
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012F4DB-A116-BF42-A76B-596179DDC028}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71569D30-A559-E742-B384-10338B5F4C96}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <t>Travail en groupe</t>
   </si>
   <si>
-    <t>Travail en groupe via chat vocal</t>
+    <t>Rédaction d'une partie du rapport concernant la logique métier.</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1108,7 +1108,9 @@
       <c r="B50" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="8"/>
+      <c r="C50" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -1141,7 +1143,7 @@
       </c>
       <c r="C56" s="9">
         <f>SUM(C5:C55)</f>
-        <v>50.75</v>
+        <v>51.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added management for changing the default bank account. Updated WorkDiary
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5086126-3E31-BB4F-BCC0-1E3BDFD138A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7953E016-EA21-B24D-B09B-DE00C7F21450}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -179,6 +180,15 @@
   </si>
   <si>
     <t>Travail sur la connexion en groupe, travail sur le hash du password en solo. Enregistrement et connexion de l'utilisateur fonctionnent.</t>
+  </si>
+  <si>
+    <t>Semaine</t>
+  </si>
+  <si>
+    <t>Cleaning de certaines classes, mise en place des commentaires, corrections de certains bug et ajout des méthodes de création et de mise à jour à la base de données pour les classes existantes.</t>
+  </si>
+  <si>
+    <t>Gestion du changement de compte par défaut</t>
   </si>
 </sst>
 </file>
@@ -247,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -270,11 +280,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +310,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -311,6 +336,865 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7154-CC4F-AD2E-E386FB452091}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="621631760"/>
+        <c:axId val="724194768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="621631760"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724194768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="724194768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621631760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7C5DF2-9D80-3F41-9CFA-766AFBAF9AC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -587,21 +1471,21 @@
     <col min="2" max="2" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +1496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43150</v>
       </c>
@@ -622,8 +1506,12 @@
       <c r="C5" s="8">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D5" s="11">
+        <f>SUM(C5:C8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43150</v>
       </c>
@@ -633,8 +1521,9 @@
       <c r="C6" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43151</v>
       </c>
@@ -644,8 +1533,9 @@
       <c r="C7" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>43151</v>
       </c>
@@ -655,8 +1545,9 @@
       <c r="C8" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43157</v>
       </c>
@@ -666,8 +1557,12 @@
       <c r="C9" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D9" s="11">
+        <f>SUM(C9:C21)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43157</v>
       </c>
@@ -677,8 +1572,9 @@
       <c r="C10" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43158</v>
       </c>
@@ -688,8 +1584,9 @@
       <c r="C11" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43158</v>
       </c>
@@ -699,8 +1596,9 @@
       <c r="C12" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43159</v>
       </c>
@@ -710,8 +1608,9 @@
       <c r="C13" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43159</v>
       </c>
@@ -721,8 +1620,9 @@
       <c r="C14" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43160</v>
       </c>
@@ -732,8 +1632,9 @@
       <c r="C15" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>43160</v>
       </c>
@@ -743,8 +1644,9 @@
       <c r="C16" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>43160</v>
       </c>
@@ -754,8 +1656,9 @@
       <c r="C17" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>43162</v>
       </c>
@@ -765,8 +1668,9 @@
       <c r="C18" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>43162</v>
       </c>
@@ -776,8 +1680,9 @@
       <c r="C19" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>43163</v>
       </c>
@@ -787,8 +1692,9 @@
       <c r="C20" s="8">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>43163</v>
       </c>
@@ -798,8 +1704,9 @@
       <c r="C21" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>43164</v>
       </c>
@@ -809,8 +1716,12 @@
       <c r="C22" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D22" s="11">
+        <f>SUM(C22:C25)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>43164</v>
       </c>
@@ -820,8 +1731,9 @@
       <c r="C23" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>43165</v>
       </c>
@@ -831,8 +1743,9 @@
       <c r="C24" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>43170</v>
       </c>
@@ -842,8 +1755,9 @@
       <c r="C25" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>43171</v>
       </c>
@@ -853,8 +1767,12 @@
       <c r="C26" s="8">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="11">
+        <f>SUM(C26:C28)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>43171</v>
       </c>
@@ -864,8 +1782,9 @@
       <c r="C27" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>43171</v>
       </c>
@@ -875,8 +1794,9 @@
       <c r="C28" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>43178</v>
       </c>
@@ -886,8 +1806,12 @@
       <c r="C29" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D29" s="11">
+        <f>SUM(C29:C33)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>43178</v>
       </c>
@@ -897,8 +1821,9 @@
       <c r="C30" s="8">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>43182</v>
       </c>
@@ -908,8 +1833,9 @@
       <c r="C31" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>43182</v>
       </c>
@@ -919,8 +1845,9 @@
       <c r="C32" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>43184</v>
       </c>
@@ -930,8 +1857,9 @@
       <c r="C33" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>43185</v>
       </c>
@@ -941,8 +1869,12 @@
       <c r="C34" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D34" s="11">
+        <f>SUM(C34:C36)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>43185</v>
       </c>
@@ -952,8 +1884,9 @@
       <c r="C35" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>43187</v>
       </c>
@@ -963,8 +1896,9 @@
       <c r="C36" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>43195</v>
       </c>
@@ -974,8 +1908,12 @@
       <c r="C37" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="10">
+        <f>SUM(C37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>43199</v>
       </c>
@@ -985,8 +1923,12 @@
       <c r="C38" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D38" s="11">
+        <f>SUM(C38:C47)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>43199</v>
       </c>
@@ -996,8 +1938,9 @@
       <c r="C39" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43202</v>
       </c>
@@ -1007,8 +1950,9 @@
       <c r="C40" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>43202</v>
       </c>
@@ -1018,8 +1962,9 @@
       <c r="C41" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>43202</v>
       </c>
@@ -1029,8 +1974,9 @@
       <c r="C42" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>43203</v>
       </c>
@@ -1040,8 +1986,9 @@
       <c r="C43" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43203</v>
       </c>
@@ -1051,8 +1998,9 @@
       <c r="C44" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>43203</v>
       </c>
@@ -1062,8 +2010,9 @@
       <c r="C45" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>43204</v>
       </c>
@@ -1073,8 +2022,9 @@
       <c r="C46" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>43205</v>
       </c>
@@ -1084,8 +2034,9 @@
       <c r="C47" s="8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>43208</v>
       </c>
@@ -1095,8 +2046,12 @@
       <c r="C48" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="10">
+        <f>SUM(C48)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>43213</v>
       </c>
@@ -1106,8 +2061,12 @@
       <c r="C49" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="11">
+        <f>SUM(C49:C51)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>43219</v>
       </c>
@@ -1117,8 +2076,9 @@
       <c r="C50" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>43219</v>
       </c>
@@ -1128,8 +2088,9 @@
       <c r="C51" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>43220</v>
       </c>
@@ -1140,35 +2101,269 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="8"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="8"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>43221</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>43222</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="5" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B76" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="9">
-        <f>SUM(C5:C55)</f>
-        <v>57</v>
+      <c r="C76" s="9">
+        <f>SUM(C5:C75)</f>
+        <v>60.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="9">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="D9:D21"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D38:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D5" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553648B4-7675-E94A-BD18-60A9A7D32F28}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>SUM(Feuil1!C5:C8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>SUM(Feuil1!C9:C21)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>SUM(Feuil1!C22:C25)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>SUM(Feuil1!C26:C28)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>SUM(Feuil1!C29:C33)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>SUM(Feuil1!C34:C36)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>SUM(Feuil1!C37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>SUM(Feuil1!C38:C47)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>SUM(Feuil1!C48)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>SUM(Feuil1!C49:C51)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated hashmap for transactions
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFADF7F-2181-9348-9C58-57442A3EBC05}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ABA5B2-3EA2-8843-8DC5-953CFF9C5E74}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Corrections de bugs pour faire fonctionner la suppression et la modification des catégories dans la db.</t>
+  </si>
+  <si>
+    <t>Préparation des méthodes pour transaction, résolutions de certains problèmes avec l'équipe et Guillaume.</t>
   </si>
 </sst>
 </file>
@@ -1475,7 +1478,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2176,13 +2179,21 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="8"/>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>43227</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
+      <c r="A59" s="3">
+        <v>43227</v>
+      </c>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
     </row>
@@ -2272,7 +2283,7 @@
       </c>
       <c r="C76" s="9">
         <f>SUM(C5:C75)</f>
-        <v>68.150000000000006</v>
+        <v>69.650000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected date.getYear bad use
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD41C1F3-3E5D-2749-9D22-69BC3A204031}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B598203-FF48-4745-A96A-7ACD5A82C27F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Travail avec François pour mettre en place les transactions. Problème lié à la fk de budget_id, impossible de toruver la cause…</t>
+  </si>
+  <si>
+    <t>Correction du bug lié à l'ajout de transactions et amélioration de la génération de la hashmap contenant les transactions.</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1484,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2204,10 +2207,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="8"/>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>43228</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
@@ -2290,7 +2299,7 @@
       </c>
       <c r="C76" s="9">
         <f>SUM(C5:C75)</f>
-        <v>71.650000000000006</v>
+        <v>73.650000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added method to retrieve all users. Added method to suppress user
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B598203-FF48-4745-A96A-7ACD5A82C27F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DBAF36-BF64-A749-9D3D-1DF69EBCB2EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Correction du bug lié à l'ajout de transactions et amélioration de la génération de la hashmap contenant les transactions.</t>
+  </si>
+  <si>
+    <t>Préparation pour la mise en place de la db derby. Corrections en ce qui concerne les transactions (modifications / suppressions) qui n'étaient pas mises à jour lors d'actions. Création d'un hashmap des transactions par catégories. Implémentation, dans Authentication, d'une fonction de déconnexion (qui s'occupe de remettre tout à zéro localement). Gestion de suppression des catégories dans les trnasactions concernées.</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2218,10 +2221,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="8"/>
+    <row r="61" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
@@ -2299,7 +2308,7 @@
       </c>
       <c r="C76" s="9">
         <f>SUM(C5:C75)</f>
-        <v>73.650000000000006</v>
+        <v>78.650000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated IOTransaction for shared budgets
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A68867-6D05-A140-AC4D-0099C71D131A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4AD6F4-ACA1-D34C-AB43-B93594A866A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>Mise en place et implémentation des classes DebtModel et DebtLogic pour la gestion des dettes. Presque tout implémenter, manque deux trois détails</t>
+  </si>
+  <si>
+    <t>Implémentation de quelques fonctions demandées par la GUI pour les dettes / budgets</t>
+  </si>
+  <si>
+    <t>Merge de la branche master dans la branch fb-derby pour mettre à jour et implémenter la fin de derby</t>
+  </si>
+  <si>
+    <t>Corrections dans quelques problèmes dans la bll</t>
   </si>
 </sst>
 </file>
@@ -429,12 +438,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,6 +458,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1604,7 +1613,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1621,10 +1630,10 @@
       <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1656,11 +1665,11 @@
       <c r="C5" s="12">
         <v>0.75</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="27">
         <f>SUM(C5:C8)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1674,8 +1683,8 @@
       <c r="C6" s="12">
         <v>0.25</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
@@ -1687,8 +1696,8 @@
       <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -1700,8 +1709,8 @@
       <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
@@ -1713,11 +1722,11 @@
       <c r="C9" s="15">
         <v>0.5</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="20">
         <f>SUM(C9:C21)</f>
         <v>15.5</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>2</v>
       </c>
     </row>
@@ -1731,8 +1740,8 @@
       <c r="C10" s="15">
         <v>0.5</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="27"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
@@ -1744,8 +1753,8 @@
       <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="27"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
@@ -1757,8 +1766,8 @@
       <c r="C12" s="15">
         <v>0.5</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="27"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
@@ -1770,8 +1779,8 @@
       <c r="C13" s="15">
         <v>0.5</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="27"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
@@ -1783,8 +1792,8 @@
       <c r="C14" s="15">
         <v>1.5</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="27"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
@@ -1796,8 +1805,8 @@
       <c r="C15" s="15">
         <v>0.5</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="27"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
@@ -1809,8 +1818,8 @@
       <c r="C16" s="15">
         <v>0.25</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="27"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
@@ -1822,8 +1831,8 @@
       <c r="C17" s="15">
         <v>1.5</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="27"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
@@ -1835,8 +1844,8 @@
       <c r="C18" s="15">
         <v>0.25</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="27"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
@@ -1848,8 +1857,8 @@
       <c r="C19" s="15">
         <v>2</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="27"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
@@ -1861,8 +1870,8 @@
       <c r="C20" s="15">
         <v>4.5</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="27"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
@@ -1874,8 +1883,8 @@
       <c r="C21" s="15">
         <v>2</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="28"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
@@ -1887,11 +1896,11 @@
       <c r="C22" s="12">
         <v>3</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="27">
         <f>SUM(C22:C25)</f>
         <v>4.25</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="21">
         <v>3</v>
       </c>
     </row>
@@ -1905,8 +1914,8 @@
       <c r="C23" s="12">
         <v>0.25</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
@@ -1918,8 +1927,8 @@
       <c r="C24" s="12">
         <v>0.5</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
@@ -1931,8 +1940,8 @@
       <c r="C25" s="12">
         <v>0.5</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="25"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
@@ -1944,11 +1953,11 @@
       <c r="C26" s="15">
         <v>0.75</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="20">
         <f>SUM(C26:C28)</f>
         <v>2.25</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1962,8 +1971,8 @@
       <c r="C27" s="15">
         <v>0.5</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="27"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
@@ -1975,8 +1984,8 @@
       <c r="C28" s="15">
         <v>1</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="28"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
@@ -1988,11 +1997,11 @@
       <c r="C29" s="12">
         <v>3</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="27">
         <f>SUM(C29:C33)</f>
         <v>7</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="21">
         <v>5</v>
       </c>
     </row>
@@ -2006,8 +2015,8 @@
       <c r="C30" s="12">
         <v>1.75</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="24"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
@@ -2019,8 +2028,8 @@
       <c r="C31" s="12">
         <v>1.5</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="24"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
@@ -2032,8 +2041,8 @@
       <c r="C32" s="12">
         <v>0.5</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="24"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
@@ -2045,8 +2054,8 @@
       <c r="C33" s="12">
         <v>0.25</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="25"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
@@ -2058,11 +2067,11 @@
       <c r="C34" s="15">
         <v>0.25</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="20">
         <f>SUM(C34:C36)</f>
         <v>3.25</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="24">
         <v>6</v>
       </c>
     </row>
@@ -2076,8 +2085,8 @@
       <c r="C35" s="15">
         <v>1.5</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="27"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
@@ -2089,8 +2098,8 @@
       <c r="C36" s="15">
         <v>1.5</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="28"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
@@ -2120,11 +2129,11 @@
       <c r="C38" s="15">
         <v>0.5</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="20">
         <f>SUM(C38:C47)</f>
         <v>10.5</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="24">
         <v>8</v>
       </c>
     </row>
@@ -2138,8 +2147,8 @@
       <c r="C39" s="15">
         <v>2</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="27"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="25"/>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
@@ -2151,8 +2160,8 @@
       <c r="C40" s="15">
         <v>2</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="27"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="25"/>
     </row>
     <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
@@ -2164,8 +2173,8 @@
       <c r="C41" s="15">
         <v>0.5</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="25"/>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
@@ -2177,8 +2186,8 @@
       <c r="C42" s="15">
         <v>1</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="27"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="25"/>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
@@ -2190,8 +2199,8 @@
       <c r="C43" s="15">
         <v>1</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="27"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="25"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
@@ -2203,8 +2212,8 @@
       <c r="C44" s="15">
         <v>0.25</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="27"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="25"/>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="13">
@@ -2216,8 +2225,8 @@
       <c r="C45" s="15">
         <v>1.5</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="27"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
@@ -2229,8 +2238,8 @@
       <c r="C46" s="15">
         <v>1.5</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="27"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
@@ -2242,8 +2251,8 @@
       <c r="C47" s="15">
         <v>0.25</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="28"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="26"/>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
@@ -2273,11 +2282,11 @@
       <c r="C49" s="15">
         <v>1.5</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="20">
         <f>SUM(C49:C51)</f>
         <v>4</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="24">
         <v>10</v>
       </c>
     </row>
@@ -2291,8 +2300,8 @@
       <c r="C50" s="15">
         <v>0.5</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="27"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
@@ -2304,8 +2313,8 @@
       <c r="C51" s="15">
         <v>2</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="28"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="26"/>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
@@ -2317,11 +2326,11 @@
       <c r="C52" s="12">
         <v>3.75</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="27">
         <f>SUM(C52:C56)</f>
         <v>12.75</v>
       </c>
-      <c r="E52" s="23">
+      <c r="E52" s="21">
         <v>11</v>
       </c>
     </row>
@@ -2335,8 +2344,8 @@
       <c r="C53" s="12">
         <v>3</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="24"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="10">
@@ -2348,8 +2357,8 @@
       <c r="C54" s="12">
         <v>0.5</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="24"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
@@ -2361,8 +2370,8 @@
       <c r="C55" s="12">
         <v>4</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="24"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
@@ -2374,8 +2383,8 @@
       <c r="C56" s="12">
         <v>1.5</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="25"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="13">
@@ -2387,11 +2396,11 @@
       <c r="C57" s="15">
         <v>2.25</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="20">
         <f>SUM(C57:C62)</f>
         <v>15.5</v>
       </c>
-      <c r="E57" s="26">
+      <c r="E57" s="24">
         <v>12</v>
       </c>
     </row>
@@ -2405,8 +2414,8 @@
       <c r="C58" s="15">
         <v>1.5</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="27"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="25"/>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="13">
@@ -2418,8 +2427,8 @@
       <c r="C59" s="15">
         <v>2</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="27"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="25"/>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="13">
@@ -2431,8 +2440,8 @@
       <c r="C60" s="15">
         <v>2</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="27"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="25"/>
     </row>
     <row r="61" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
@@ -2444,8 +2453,8 @@
       <c r="C61" s="15">
         <v>5</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="27"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="13">
@@ -2457,8 +2466,8 @@
       <c r="C62" s="15">
         <v>2.75</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="28"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="26"/>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
@@ -2493,20 +2502,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="8"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="8"/>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="8"/>
+      <c r="A68" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
@@ -2549,11 +2576,20 @@
       </c>
       <c r="C76" s="9">
         <f>SUM(C5:C75)</f>
-        <v>85.5</v>
+        <v>89.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="D9:D21"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D38:D47"/>
     <mergeCell ref="D57:D62"/>
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="E9:E21"/>
@@ -2566,15 +2602,6 @@
     <mergeCell ref="E52:E56"/>
     <mergeCell ref="E57:E62"/>
     <mergeCell ref="D52:D56"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="D9:D21"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D38:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Little commit. No importance
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Daniel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD96EF1A-7A7C-324B-BE75-7105647F1ED7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09EE0D-2C61-B24D-93B3-3FB6FD605A45}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -239,7 +239,10 @@
     <t>Corrections de quelques problèmes dans la bll</t>
   </si>
   <si>
-    <t>Travail en groupe pour faire fonctionner les budgets, les budgets partagés et les dettes. Quelques bugs restent à corriger, mais presquefini.</t>
+    <t>Travail en groupe pour faire fonctionner les budgets, les budgets partagés et les dettes. Quelques bugs restent à corriger, mais presque fini.</t>
+  </si>
+  <si>
+    <t>Mis à jour de la branche fb-derby avec la branche master, on doit encore vérifier que tout marche avec Derby puis on merge les deux branches. On a essayer de créer le jar avec Guillaume, pas réussi. Problème de manifest, on check plus tard.</t>
   </si>
 </sst>
 </file>
@@ -441,6 +444,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,12 +470,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1616,7 +1619,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1633,10 +1636,10 @@
       <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1668,11 +1671,11 @@
       <c r="C5" s="12">
         <v>0.75</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="21">
         <f>SUM(C5:C8)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1686,8 +1689,8 @@
       <c r="C6" s="12">
         <v>0.25</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
@@ -1699,8 +1702,8 @@
       <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -1712,8 +1715,8 @@
       <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
@@ -1725,11 +1728,11 @@
       <c r="C9" s="15">
         <v>0.5</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="22">
         <f>SUM(C9:C21)</f>
         <v>15.5</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="26">
         <v>2</v>
       </c>
     </row>
@@ -1743,8 +1746,8 @@
       <c r="C10" s="15">
         <v>0.5</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
@@ -1756,8 +1759,8 @@
       <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="25"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
@@ -1769,8 +1772,8 @@
       <c r="C12" s="15">
         <v>0.5</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="25"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
@@ -1782,8 +1785,8 @@
       <c r="C13" s="15">
         <v>0.5</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
@@ -1795,8 +1798,8 @@
       <c r="C14" s="15">
         <v>1.5</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
@@ -1808,8 +1811,8 @@
       <c r="C15" s="15">
         <v>0.5</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="25"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
@@ -1821,8 +1824,8 @@
       <c r="C16" s="15">
         <v>0.25</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="25"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
@@ -1834,8 +1837,8 @@
       <c r="C17" s="15">
         <v>1.5</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="25"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
@@ -1847,8 +1850,8 @@
       <c r="C18" s="15">
         <v>0.25</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="25"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
@@ -1860,8 +1863,8 @@
       <c r="C19" s="15">
         <v>2</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="25"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
@@ -1873,8 +1876,8 @@
       <c r="C20" s="15">
         <v>4.5</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="25"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
@@ -1886,8 +1889,8 @@
       <c r="C21" s="15">
         <v>2</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="26"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
@@ -1899,11 +1902,11 @@
       <c r="C22" s="12">
         <v>3</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="21">
         <f>SUM(C22:C25)</f>
         <v>4.25</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1917,8 +1920,8 @@
       <c r="C23" s="12">
         <v>0.25</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
@@ -1930,8 +1933,8 @@
       <c r="C24" s="12">
         <v>0.5</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
@@ -1943,8 +1946,8 @@
       <c r="C25" s="12">
         <v>0.5</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="23"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
@@ -1956,11 +1959,11 @@
       <c r="C26" s="15">
         <v>0.75</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="22">
         <f>SUM(C26:C28)</f>
         <v>2.25</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="26">
         <v>4</v>
       </c>
     </row>
@@ -1974,8 +1977,8 @@
       <c r="C27" s="15">
         <v>0.5</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="25"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
@@ -1987,8 +1990,8 @@
       <c r="C28" s="15">
         <v>1</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="26"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
@@ -2000,11 +2003,11 @@
       <c r="C29" s="12">
         <v>3</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="21">
         <f>SUM(C29:C33)</f>
         <v>7</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="23">
         <v>5</v>
       </c>
     </row>
@@ -2018,8 +2021,8 @@
       <c r="C30" s="12">
         <v>1.75</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="22"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
@@ -2031,8 +2034,8 @@
       <c r="C31" s="12">
         <v>1.5</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="22"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="24"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
@@ -2044,8 +2047,8 @@
       <c r="C32" s="12">
         <v>0.5</v>
       </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="22"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
@@ -2057,8 +2060,8 @@
       <c r="C33" s="12">
         <v>0.25</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
@@ -2070,11 +2073,11 @@
       <c r="C34" s="15">
         <v>0.25</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="22">
         <f>SUM(C34:C36)</f>
         <v>3.25</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="26">
         <v>6</v>
       </c>
     </row>
@@ -2088,8 +2091,8 @@
       <c r="C35" s="15">
         <v>1.5</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="25"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
@@ -2101,8 +2104,8 @@
       <c r="C36" s="15">
         <v>1.5</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="26"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
@@ -2132,11 +2135,11 @@
       <c r="C38" s="15">
         <v>0.5</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="22">
         <f>SUM(C38:C47)</f>
         <v>10.5</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="26">
         <v>8</v>
       </c>
     </row>
@@ -2150,8 +2153,8 @@
       <c r="C39" s="15">
         <v>2</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="25"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="27"/>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
@@ -2163,8 +2166,8 @@
       <c r="C40" s="15">
         <v>2</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="25"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
@@ -2176,8 +2179,8 @@
       <c r="C41" s="15">
         <v>0.5</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="25"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
@@ -2189,8 +2192,8 @@
       <c r="C42" s="15">
         <v>1</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="25"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="27"/>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
@@ -2202,8 +2205,8 @@
       <c r="C43" s="15">
         <v>1</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="25"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
@@ -2215,8 +2218,8 @@
       <c r="C44" s="15">
         <v>0.25</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="25"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="13">
@@ -2228,8 +2231,8 @@
       <c r="C45" s="15">
         <v>1.5</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="25"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
@@ -2241,8 +2244,8 @@
       <c r="C46" s="15">
         <v>1.5</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="25"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
@@ -2254,8 +2257,8 @@
       <c r="C47" s="15">
         <v>0.25</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="26"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
@@ -2285,11 +2288,11 @@
       <c r="C49" s="15">
         <v>1.5</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D49" s="22">
         <f>SUM(C49:C51)</f>
         <v>4</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="26">
         <v>10</v>
       </c>
     </row>
@@ -2303,8 +2306,8 @@
       <c r="C50" s="15">
         <v>0.5</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="25"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="27"/>
     </row>
     <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
@@ -2316,8 +2319,8 @@
       <c r="C51" s="15">
         <v>2</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="26"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="28"/>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
@@ -2329,11 +2332,11 @@
       <c r="C52" s="12">
         <v>3.75</v>
       </c>
-      <c r="D52" s="27">
+      <c r="D52" s="21">
         <f>SUM(C52:C56)</f>
         <v>12.75</v>
       </c>
-      <c r="E52" s="21">
+      <c r="E52" s="23">
         <v>11</v>
       </c>
     </row>
@@ -2347,8 +2350,8 @@
       <c r="C53" s="12">
         <v>3</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="22"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="10">
@@ -2360,8 +2363,8 @@
       <c r="C54" s="12">
         <v>0.5</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="22"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="24"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
@@ -2373,8 +2376,8 @@
       <c r="C55" s="12">
         <v>4</v>
       </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="22"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="24"/>
     </row>
     <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
@@ -2386,8 +2389,8 @@
       <c r="C56" s="12">
         <v>1.5</v>
       </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="23"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="25"/>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="13">
@@ -2399,11 +2402,11 @@
       <c r="C57" s="15">
         <v>2.25</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="22">
         <f>SUM(C57:C62)</f>
         <v>15.5</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="26">
         <v>12</v>
       </c>
     </row>
@@ -2417,8 +2420,8 @@
       <c r="C58" s="15">
         <v>1.5</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="25"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="13">
@@ -2430,8 +2433,8 @@
       <c r="C59" s="15">
         <v>2</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="25"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="27"/>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="13">
@@ -2443,8 +2446,8 @@
       <c r="C60" s="15">
         <v>2</v>
       </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="25"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="27"/>
     </row>
     <row r="61" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
@@ -2456,8 +2459,8 @@
       <c r="C61" s="15">
         <v>5</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="25"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="13">
@@ -2469,8 +2472,8 @@
       <c r="C62" s="15">
         <v>2.75</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="26"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="28"/>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
@@ -2549,10 +2552,16 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="8"/>
+    <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>43238</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="8">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
@@ -2585,20 +2594,11 @@
       </c>
       <c r="C76" s="9">
         <f>SUM(C5:C75)</f>
-        <v>93.25</v>
+        <v>94.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="D9:D21"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D38:D47"/>
     <mergeCell ref="D57:D62"/>
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="E9:E21"/>
@@ -2611,6 +2611,15 @@
     <mergeCell ref="E52:E56"/>
     <mergeCell ref="E57:E62"/>
     <mergeCell ref="D52:D56"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="D9:D21"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D38:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>